<commit_message>
Updated script and mapping files
Updates to script, better handling of person entities and removed appellation instances
</commit_message>
<xml_diff>
--- a/mapping1.xlsx
+++ b/mapping1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C6A506-D21E-49AB-8657-1F89AF29DD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E0AB32-1F37-4840-AF63-1B27D793E2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="132">
   <si>
     <t>Subject</t>
   </si>
@@ -196,18 +196,12 @@
     <t>rico:identifier</t>
   </si>
   <si>
-    <t>rico:hasOrHadAppellation</t>
-  </si>
-  <si>
     <t>has value</t>
   </si>
   <si>
     <t>rdf:value</t>
   </si>
   <si>
-    <t>has type</t>
-  </si>
-  <si>
     <t>Data 1934</t>
   </si>
   <si>
@@ -262,15 +256,9 @@
     <t>Person Francesco Acri</t>
   </si>
   <si>
-    <t>Person</t>
-  </si>
-  <si>
     <t>Persona URI</t>
   </si>
   <si>
-    <t>rico:Person</t>
-  </si>
-  <si>
     <t>has sender</t>
   </si>
   <si>
@@ -325,15 +313,6 @@
     <t>mittenti extra</t>
   </si>
   <si>
-    <t>VIAF extra</t>
-  </si>
-  <si>
-    <t>Medea Norsa</t>
-  </si>
-  <si>
-    <t>http://viaf.org/viaf/66589736</t>
-  </si>
-  <si>
     <t>rico:RecordSet</t>
   </si>
   <si>
@@ -449,6 +428,15 @@
   </si>
   <si>
     <t>rico:hasOrHadIdentifier</t>
+  </si>
+  <si>
+    <t>has_title</t>
+  </si>
+  <si>
+    <t>Acri, Francesco</t>
+  </si>
+  <si>
+    <t>rdfs:label</t>
   </si>
 </sst>
 </file>
@@ -875,7 +863,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +921,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -964,10 +952,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>10</v>
@@ -990,7 +978,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
@@ -1007,19 +995,19 @@
         <v>49</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>10</v>
@@ -1033,19 +1021,19 @@
         <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
@@ -1059,19 +1047,19 @@
         <v>49</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>10</v>
@@ -1088,39 +1076,39 @@
         <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="5">
         <v>1934</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>15</v>
@@ -1133,16 +1121,16 @@
         <v>49</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>15</v>
@@ -1162,13 +1150,13 @@
         <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>15</v>
@@ -1190,7 +1178,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,7 +1236,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -1257,7 +1245,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1272,7 +1260,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -1281,7 +1269,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>29</v>
@@ -1293,10 +1281,10 @@
         <v>26</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>28</v>
@@ -1307,7 +1295,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>27</v>
@@ -1319,10 +1307,10 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>28</v>
@@ -1339,7 +1327,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>25</v>
@@ -1348,7 +1336,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>25</v>
@@ -1359,7 +1347,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>13</v>
@@ -1371,10 +1359,10 @@
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
@@ -1385,97 +1373,97 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>15</v>
@@ -1489,19 +1477,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>15</v>
@@ -1515,28 +1503,28 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1550,7 +1538,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,7 +1595,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -1616,7 +1604,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1631,7 +1619,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -1640,7 +1628,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -1655,7 +1643,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -1664,7 +1652,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>29</v>
@@ -1676,10 +1664,10 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>28</v>
@@ -1690,7 +1678,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>29</v>
@@ -1702,10 +1690,10 @@
         <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>31</v>
@@ -1716,7 +1704,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>27</v>
@@ -1728,10 +1716,10 @@
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
@@ -1742,22 +1730,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>31</v>
@@ -1768,7 +1756,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>13</v>
@@ -1780,7 +1768,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>15</v>
@@ -1794,7 +1782,7 @@
     </row>
     <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>36</v>
@@ -1806,7 +1794,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>15</v>
@@ -1825,10 +1813,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5079B550-D5DB-4565-A3E4-EB975460C499}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,7 +1873,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -1894,7 +1882,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1909,7 +1897,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -1918,7 +1906,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -1933,7 +1921,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -1942,7 +1930,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -1957,7 +1945,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>40</v>
@@ -1978,10 +1966,10 @@
         <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>10</v>
@@ -1992,7 +1980,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>29</v>
@@ -2018,7 +2006,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
@@ -2044,7 +2032,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -2056,10 +2044,10 @@
         <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>40</v>
@@ -2070,7 +2058,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>13</v>
@@ -2082,7 +2070,7 @@
         <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>15</v>
@@ -2096,22 +2084,22 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>40</v>
@@ -2122,22 +2110,22 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>40</v>
@@ -2148,22 +2136,22 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>40</v>
@@ -2174,22 +2162,22 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>40</v>
@@ -2200,19 +2188,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>15</v>
@@ -2225,47 +2213,33 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>40</v>
@@ -2276,13 +2250,13 @@
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>46</v>
@@ -2299,6 +2273,16 @@
       <c r="H18" s="4" t="s">
         <v>45</v>
       </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2310,10 +2294,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF64A34-3DF9-46D7-BC95-3BB1594FAE3C}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD11"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2370,7 +2354,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -2379,7 +2363,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -2394,7 +2378,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -2403,7 +2387,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -2418,7 +2402,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -2427,7 +2411,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -2442,7 +2426,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>40</v>
@@ -2451,25 +2435,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -2487,10 +2471,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
@@ -2501,7 +2485,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
@@ -2513,10 +2497,10 @@
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>28</v>
@@ -2527,7 +2511,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -2539,10 +2523,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>31</v>
@@ -2553,7 +2537,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>29</v>
@@ -2565,10 +2549,10 @@
         <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>40</v>
@@ -2579,210 +2563,210 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="F17" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2797,112 +2781,105 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="C20" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>93</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="E22" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="H22" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>45</v>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C23" r:id="rId1" xr:uid="{1F845F2E-9258-4F48-AD04-C46E732165E5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2911,7 +2888,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2969,7 +2946,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -2978,7 +2955,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -2993,7 +2970,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -3002,7 +2979,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -3017,7 +2994,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -3026,7 +3003,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -3041,7 +3018,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>40</v>
@@ -3050,25 +3027,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -3086,10 +3063,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
@@ -3100,7 +3077,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
@@ -3112,10 +3089,10 @@
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>28</v>
@@ -3126,7 +3103,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -3138,10 +3115,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>31</v>
@@ -3152,7 +3129,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>29</v>
@@ -3164,10 +3141,10 @@
         <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>40</v>
@@ -3178,80 +3155,80 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated mapping and added umls
</commit_message>
<xml_diff>
--- a/mapping1.xlsx
+++ b/mapping1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Stage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E0AB32-1F37-4840-AF63-1B27D793E2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983AFDB3-5B28-46EE-97A0-400EC2BF817B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Serie" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="131">
   <si>
     <t>Subject</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>Serie S1</t>
-  </si>
-  <si>
-    <t>rico:identifier</t>
   </si>
   <si>
     <t>has value</t>
@@ -862,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,7 +918,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -952,10 +949,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>10</v>
@@ -978,7 +975,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
@@ -995,19 +992,19 @@
         <v>49</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>10</v>
@@ -1021,19 +1018,19 @@
         <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
@@ -1047,19 +1044,19 @@
         <v>49</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>10</v>
@@ -1076,39 +1073,39 @@
         <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5">
         <v>1934</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>15</v>
@@ -1121,16 +1118,16 @@
         <v>49</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>15</v>
@@ -1150,13 +1147,13 @@
         <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>15</v>
@@ -1236,7 +1233,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -1245,7 +1242,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1260,7 +1257,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -1269,7 +1266,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>29</v>
@@ -1281,10 +1278,10 @@
         <v>26</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>28</v>
@@ -1295,7 +1292,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>27</v>
@@ -1307,10 +1304,10 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>28</v>
@@ -1327,7 +1324,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>25</v>
@@ -1336,7 +1333,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>25</v>
@@ -1347,7 +1344,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>13</v>
@@ -1359,10 +1356,10 @@
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
@@ -1373,97 +1370,97 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>15</v>
@@ -1477,19 +1474,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>15</v>
@@ -1503,28 +1500,28 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1538,7 +1535,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,7 +1592,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -1604,7 +1601,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1619,7 +1616,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -1628,7 +1625,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -1643,7 +1640,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -1652,7 +1649,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>29</v>
@@ -1664,10 +1661,10 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>28</v>
@@ -1678,7 +1675,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>29</v>
@@ -1690,10 +1687,10 @@
         <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>31</v>
@@ -1704,7 +1701,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>27</v>
@@ -1716,10 +1713,10 @@
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
@@ -1730,22 +1727,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>31</v>
@@ -1756,7 +1753,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>13</v>
@@ -1768,7 +1765,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>15</v>
@@ -1782,7 +1779,7 @@
     </row>
     <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>36</v>
@@ -1794,7 +1791,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>15</v>
@@ -1808,6 +1805,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1815,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5079B550-D5DB-4565-A3E4-EB975460C499}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1871,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -1882,7 +1880,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1897,7 +1895,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -1906,7 +1904,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -1921,7 +1919,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -1930,7 +1928,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -1945,7 +1943,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>40</v>
@@ -1966,10 +1964,10 @@
         <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>10</v>
@@ -1980,7 +1978,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>29</v>
@@ -1992,10 +1990,10 @@
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
@@ -2006,7 +2004,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
@@ -2018,10 +2016,10 @@
         <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>31</v>
@@ -2032,7 +2030,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -2044,10 +2042,10 @@
         <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>40</v>
@@ -2058,7 +2056,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>13</v>
@@ -2070,7 +2068,7 @@
         <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>15</v>
@@ -2084,22 +2082,22 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>40</v>
@@ -2110,22 +2108,22 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>40</v>
@@ -2136,22 +2134,22 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>40</v>
@@ -2162,22 +2160,22 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>40</v>
@@ -2188,19 +2186,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>15</v>
@@ -2224,22 +2222,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>40</v>
@@ -2250,13 +2248,13 @@
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>46</v>
@@ -2296,8 +2294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF64A34-3DF9-46D7-BC95-3BB1594FAE3C}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2354,7 +2352,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -2363,7 +2361,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -2378,7 +2376,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -2387,7 +2385,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -2402,7 +2400,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -2411,7 +2409,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -2426,7 +2424,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>40</v>
@@ -2435,25 +2433,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -2471,10 +2469,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
@@ -2485,7 +2483,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
@@ -2497,10 +2495,10 @@
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>28</v>
@@ -2511,7 +2509,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -2523,10 +2521,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>31</v>
@@ -2537,7 +2535,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>29</v>
@@ -2549,10 +2547,10 @@
         <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>40</v>
@@ -2563,210 +2561,210 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="H11" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="D13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="H13" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="D14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="H14" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="F15" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="H15" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="D16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="H16" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="H17" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2781,28 +2779,28 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="H20" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2817,28 +2815,28 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="H22" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2853,28 +2851,28 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>131</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2946,7 +2944,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -2955,7 +2953,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -2970,7 +2968,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -2979,7 +2977,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -2994,7 +2992,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -3003,7 +3001,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -3018,7 +3016,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>40</v>
@@ -3027,25 +3025,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -3063,10 +3061,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
@@ -3077,7 +3075,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
@@ -3089,10 +3087,10 @@
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>28</v>
@@ -3103,7 +3101,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -3115,10 +3113,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>31</v>
@@ -3129,7 +3127,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>29</v>
@@ -3141,10 +3139,10 @@
         <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>40</v>
@@ -3155,80 +3153,80 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="H11" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated script and mapping
Added directlyincludedin relationships between documents and fascicolo, added isdirectlyincludedin relationships between documents and immagine
Added instantiation creation for record resources
</commit_message>
<xml_diff>
--- a/mapping1.xlsx
+++ b/mapping1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Internship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983AFDB3-5B28-46EE-97A0-400EC2BF817B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C66D4B-7108-4AEA-ACB0-8FAC69A6DF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Serie" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="129">
   <si>
     <t>Subject</t>
   </si>
@@ -175,24 +175,12 @@
     <t>data</t>
   </si>
   <si>
-    <t>sameAs</t>
-  </si>
-  <si>
-    <t>VIAF</t>
-  </si>
-  <si>
-    <t>Denominazione Fascicolo</t>
-  </si>
-  <si>
-    <t>OWL:sameAs</t>
-  </si>
-  <si>
-    <t>VIAF URI</t>
-  </si>
-  <si>
     <t>Serie S1</t>
   </si>
   <si>
+    <t>rico:identifier</t>
+  </si>
+  <si>
     <t>has value</t>
   </si>
   <si>
@@ -262,9 +250,6 @@
     <t>rico:hasSender</t>
   </si>
   <si>
-    <t>http://viaf.org/viaf/30343628</t>
-  </si>
-  <si>
     <t>S1_SS1_B1_001_01</t>
   </si>
   <si>
@@ -388,9 +373,6 @@
     <t>record</t>
   </si>
   <si>
-    <t>rico:Record</t>
-  </si>
-  <si>
     <t>estremi cronologici</t>
   </si>
   <si>
@@ -434,13 +416,25 @@
   </si>
   <si>
     <t>rdfs:label</t>
+  </si>
+  <si>
+    <t>rico:Date</t>
+  </si>
+  <si>
+    <t>has_instantiation</t>
+  </si>
+  <si>
+    <t>rico:hasOrHadInstantiation</t>
+  </si>
+  <si>
+    <t>rico:Instantiation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,14 +488,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -549,7 +535,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -558,10 +544,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -859,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +886,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -918,7 +901,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -926,18 +909,32 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>29</v>
@@ -949,10 +946,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>10</v>
@@ -963,7 +960,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>13</v>
@@ -975,7 +972,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>15</v>
@@ -989,22 +986,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>10</v>
@@ -1015,22 +1012,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
@@ -1041,22 +1038,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>10</v>
@@ -1067,45 +1064,45 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C10" s="5">
         <v>1934</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>15</v>
@@ -1115,19 +1112,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>15</v>
@@ -1141,19 +1138,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>15</v>
@@ -1172,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95813D3A-72E7-4BB6-8FB9-93240D7FEB11}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,7 +1215,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -1233,7 +1230,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -1242,7 +1239,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1257,7 +1254,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -1266,7 +1263,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>29</v>
@@ -1278,10 +1275,10 @@
         <v>26</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>28</v>
@@ -1292,22 +1289,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>28</v>
@@ -1324,7 +1321,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>25</v>
@@ -1333,7 +1330,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>25</v>
@@ -1344,7 +1341,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>13</v>
@@ -1356,10 +1353,10 @@
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
@@ -1370,97 +1367,97 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>15</v>
@@ -1474,19 +1471,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>15</v>
@@ -1500,29 +1497,53 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1532,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40EA28B1-050B-43BF-9433-146B7B2429F5}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,7 +1598,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -1592,7 +1613,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -1601,7 +1622,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1616,7 +1637,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -1625,7 +1646,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -1640,7 +1661,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -1649,7 +1670,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>29</v>
@@ -1661,10 +1682,10 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>28</v>
@@ -1675,7 +1696,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>29</v>
@@ -1687,10 +1708,10 @@
         <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>31</v>
@@ -1701,22 +1722,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
@@ -1727,22 +1748,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>31</v>
@@ -1753,7 +1774,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>13</v>
@@ -1765,7 +1786,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>15</v>
@@ -1777,21 +1798,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>15</v>
@@ -1803,9 +1824,32 @@
         <v>37</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1814,7 +1858,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,7 +1900,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -1871,7 +1915,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -1880,7 +1924,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1895,7 +1939,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -1904,7 +1948,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -1919,7 +1963,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -1928,7 +1972,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -1943,7 +1987,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>40</v>
@@ -1952,7 +1996,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>29</v>
@@ -1964,10 +2008,10 @@
         <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>10</v>
@@ -1978,7 +2022,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>29</v>
@@ -1990,10 +2034,10 @@
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
@@ -2004,7 +2048,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
@@ -2016,10 +2060,10 @@
         <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>31</v>
@@ -2030,7 +2074,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -2042,10 +2086,10 @@
         <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>40</v>
@@ -2056,19 +2100,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>15</v>
@@ -2082,22 +2126,22 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>40</v>
@@ -2108,22 +2152,22 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>40</v>
@@ -2134,22 +2178,22 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>40</v>
@@ -2160,22 +2204,22 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>40</v>
@@ -2186,19 +2230,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>15</v>
@@ -2222,22 +2266,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>40</v>
@@ -2246,31 +2290,29 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>73</v>
+        <v>126</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>47</v>
+        <v>127</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -2283,9 +2325,6 @@
       <c r="H19" s="4"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C18" r:id="rId1" xr:uid="{232A5D06-C4B0-427D-8CE1-8311E3C7B68F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2295,7 +2334,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2337,7 +2376,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -2352,7 +2391,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -2361,7 +2400,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -2376,7 +2415,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -2385,7 +2424,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -2400,7 +2439,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -2409,7 +2448,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -2424,7 +2463,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>40</v>
@@ -2433,31 +2472,31 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>29</v>
@@ -2469,10 +2508,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
@@ -2483,7 +2522,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
@@ -2495,10 +2534,10 @@
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>28</v>
@@ -2509,7 +2548,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -2521,10 +2560,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>31</v>
@@ -2535,7 +2574,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>29</v>
@@ -2547,10 +2586,10 @@
         <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>40</v>
@@ -2561,319 +2600,365 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>77</v>
+      <c r="C12" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="G16" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>94</v>
+      <c r="C18" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="G20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="4" t="s">
+      <c r="H22" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>88</v>
-      </c>
+      <c r="E24" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2885,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750A8FC3-B2D9-4857-BDBF-97A1C08E4AF5}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2929,7 +3014,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -2944,7 +3029,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -2953,7 +3038,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -2968,7 +3053,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>28</v>
@@ -2977,7 +3062,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -2992,7 +3077,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
@@ -3001,7 +3086,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -3016,7 +3101,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>40</v>
@@ -3025,31 +3110,31 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>29</v>
@@ -3061,10 +3146,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
@@ -3075,7 +3160,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>29</v>
@@ -3087,10 +3172,10 @@
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>28</v>
@@ -3101,7 +3186,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -3113,10 +3198,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>31</v>
@@ -3127,7 +3212,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>29</v>
@@ -3139,10 +3224,10 @@
         <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>40</v>
@@ -3153,111 +3238,155 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>104</v>
+        <v>122</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -3270,19 +3399,19 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="10"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>

</xml_diff>

<commit_message>
Updated output with new instances file
</commit_message>
<xml_diff>
--- a/mapping1.xlsx
+++ b/mapping1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF83D95-3018-4ABE-B151-FD3694B79C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EC62E6-4008-4FC6-8547-B815E87CF896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Serie" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -497,6 +497,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -513,7 +519,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -531,6 +537,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{08C24E78-6A17-4A87-A738-8B2FB3EFD137}"/>
@@ -817,22 +824,22 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.33203125" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -858,7 +865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -884,7 +891,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
@@ -910,14 +917,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="9" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -936,14 +943,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="9" t="s">
         <v>103</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -962,7 +969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>42</v>
       </c>
@@ -984,7 +991,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
@@ -1010,7 +1017,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
@@ -1046,22 +1053,22 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1087,7 +1094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
@@ -1113,7 +1120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -1139,7 +1146,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>49</v>
       </c>
@@ -1165,7 +1172,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>49</v>
       </c>
@@ -1191,7 +1198,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
@@ -1217,7 +1224,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
@@ -1243,7 +1250,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
@@ -1269,7 +1276,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>49</v>
       </c>
@@ -1295,7 +1302,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>49</v>
       </c>
@@ -1332,21 +1339,21 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1372,7 +1379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
@@ -1398,7 +1405,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
@@ -1424,7 +1431,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>105</v>
       </c>
@@ -1476,7 +1483,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>105</v>
       </c>
@@ -1502,7 +1509,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>105</v>
       </c>
@@ -1528,7 +1535,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>105</v>
       </c>
@@ -1554,7 +1561,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>55</v>
       </c>
@@ -1580,7 +1587,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
@@ -1604,7 +1611,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>55</v>
       </c>
@@ -1638,21 +1645,21 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1678,7 +1685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
@@ -1704,7 +1711,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>106</v>
       </c>
@@ -1730,7 +1737,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>106</v>
       </c>
@@ -1756,7 +1763,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>106</v>
       </c>
@@ -1782,7 +1789,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>106</v>
       </c>
@@ -1808,7 +1815,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
@@ -1834,7 +1841,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>79</v>
       </c>
@@ -1860,7 +1867,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>66</v>
       </c>
@@ -1886,7 +1893,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
@@ -1910,7 +1917,7 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>66</v>
       </c>
@@ -1936,7 +1943,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
@@ -1962,7 +1969,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>66</v>
       </c>
@@ -1997,22 +2004,22 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2038,7 +2045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -2062,7 +2069,7 @@
       </c>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>49</v>
       </c>
@@ -2086,7 +2093,7 @@
       </c>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
@@ -2110,7 +2117,7 @@
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>82</v>
       </c>
@@ -2134,7 +2141,7 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>83</v>
       </c>
@@ -2158,7 +2165,7 @@
       </c>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
@@ -2184,7 +2191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
@@ -2210,7 +2217,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
@@ -2236,7 +2243,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
@@ -2262,7 +2269,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>67</v>
       </c>
@@ -2288,7 +2295,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>83</v>
       </c>
@@ -2314,7 +2321,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>83</v>
       </c>
@@ -2340,7 +2347,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>67</v>
       </c>
@@ -2364,7 +2371,7 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>83</v>
       </c>
@@ -2390,7 +2397,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>

</xml_diff>